<commit_message>
block intermediate action, clear data on action completed
</commit_message>
<xml_diff>
--- a/century_spice.xlsx
+++ b/century_spice.xlsx
@@ -9,12 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21525" windowHeight="12405"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21525" windowHeight="12405" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Score Card" sheetId="1" r:id="rId1"/>
     <sheet name="Trade Card" sheetId="2" r:id="rId2"/>
-    <sheet name="Start Card" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -542,7 +541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2:I37"/>
     </sheetView>
   </sheetViews>
@@ -1629,8 +1628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V45"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3:V45"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="U45" sqref="A45:U45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -3669,17 +3668,4 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
-  <sheetData/>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>